<commit_message>
support for split in <>
</commit_message>
<xml_diff>
--- a/sweetest/element/Baidu-Elements.xlsx
+++ b/sweetest/element/Baidu-Elements.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
   <si>
     <t>page</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -253,38 +253,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>项目状态#</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sonar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>element</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>baseurl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>custom</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>headers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>config</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>登录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http#</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -293,23 +273,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>api/qualitygates/project_status?projectKey=#</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://vwt-sonar/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>api/authentication/login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'Content-Type':'application/x-www-form-urlencoded'}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>select STKPOOLID,STKID,STKNAME from ir_stkpool_member_etl where STKPOOLID='#'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alert#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>custom 列一般用作页面有 frame 的情况，如果元素不在默认 frame，需要填写该元素的 frame id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在同一个 page 层级下，下层元素的 custom 自动继承上一个元素的值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>灰色背景的行，为通用预定义元素，请勿删除</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -320,30 +308,6 @@
 password=123456,
 dbname=test,
 sid=jzdb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>alert</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>alert#</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>custom 列一般用作页面有 frame 的情况，如果元素不在默认 frame，需要填写该元素的 frame id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在同一个 page 层级下，下层元素的 custom 自动继承上一个元素的值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>灰色背景的行，为通用预定义元素，请勿删除</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -536,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -558,12 +522,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -906,11 +864,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -928,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -937,7 +895,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
@@ -956,7 +914,7 @@
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -970,23 +928,23 @@
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="10" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1158,11 +1116,11 @@
     <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="3"/>
@@ -1260,11 +1218,11 @@
         <v>55</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1276,7 +1234,7 @@
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="5" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1294,52 +1252,34 @@
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="12"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="12"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
-      <c r="B29" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
-      <c r="B30" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="B30" s="5"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="D30" s="5"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
@@ -1380,119 +1320,119 @@
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
+      <c r="A36" s="6"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
+      <c r="A37" s="6"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
+      <c r="A38" s="6"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
+      <c r="A39" s="6"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
+      <c r="A40" s="7"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="13"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="12"/>
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="3"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="13"/>
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="3"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="9"/>
       <c r="E42" s="13"/>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="4"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="6"/>
     </row>
     <row r="44" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
+      <c r="A44" s="6"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="8"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="3"/>
       <c r="E44" s="14"/>
-      <c r="F44" s="4"/>
+      <c r="F44" s="6"/>
     </row>
     <row r="45" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="6"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="4"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="6"/>
     </row>
     <row r="46" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A46" s="7"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="9"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="15"/>
-      <c r="F46" s="4"/>
+      <c r="F46" s="6"/>
     </row>
     <row r="47" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
+      <c r="A47" s="6"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="7"/>
+      <c r="C47" s="6"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="16"/>
+      <c r="E47" s="14"/>
       <c r="F47" s="6"/>
     </row>
     <row r="48" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="5"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="16"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="15"/>
       <c r="F48" s="6"/>
     </row>
     <row r="49" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="3"/>
-      <c r="C49" s="7"/>
+      <c r="C49" s="6"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="16"/>
+      <c r="E49" s="14"/>
       <c r="F49" s="6"/>
     </row>
     <row r="50" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1500,7 +1440,7 @@
       <c r="B50" s="5"/>
       <c r="C50" s="6"/>
       <c r="D50" s="5"/>
-      <c r="E50" s="17"/>
+      <c r="E50" s="15"/>
       <c r="F50" s="6"/>
     </row>
     <row r="51" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1508,7 +1448,7 @@
       <c r="B51" s="3"/>
       <c r="C51" s="6"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="16"/>
+      <c r="E51" s="14"/>
       <c r="F51" s="6"/>
     </row>
     <row r="52" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1516,7 +1456,7 @@
       <c r="B52" s="5"/>
       <c r="C52" s="6"/>
       <c r="D52" s="5"/>
-      <c r="E52" s="17"/>
+      <c r="E52" s="15"/>
       <c r="F52" s="6"/>
     </row>
     <row r="53" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1524,7 +1464,7 @@
       <c r="B53" s="3"/>
       <c r="C53" s="6"/>
       <c r="D53" s="3"/>
-      <c r="E53" s="16"/>
+      <c r="E53" s="14"/>
       <c r="F53" s="6"/>
     </row>
     <row r="54" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1532,7 +1472,7 @@
       <c r="B54" s="5"/>
       <c r="C54" s="6"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="17"/>
+      <c r="E54" s="15"/>
       <c r="F54" s="6"/>
     </row>
     <row r="55" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1540,7 +1480,7 @@
       <c r="B55" s="3"/>
       <c r="C55" s="6"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="16"/>
+      <c r="E55" s="14"/>
       <c r="F55" s="6"/>
     </row>
     <row r="56" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1548,7 +1488,7 @@
       <c r="B56" s="5"/>
       <c r="C56" s="6"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="17"/>
+      <c r="E56" s="15"/>
       <c r="F56" s="6"/>
     </row>
     <row r="57" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1556,7 +1496,7 @@
       <c r="B57" s="3"/>
       <c r="C57" s="6"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="16"/>
+      <c r="E57" s="14"/>
       <c r="F57" s="6"/>
     </row>
     <row r="58" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1564,7 +1504,7 @@
       <c r="B58" s="5"/>
       <c r="C58" s="6"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="17"/>
+      <c r="E58" s="15"/>
       <c r="F58" s="6"/>
     </row>
     <row r="59" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1572,7 +1512,7 @@
       <c r="B59" s="3"/>
       <c r="C59" s="6"/>
       <c r="D59" s="3"/>
-      <c r="E59" s="16"/>
+      <c r="E59" s="14"/>
       <c r="F59" s="6"/>
     </row>
     <row r="60" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1580,7 +1520,7 @@
       <c r="B60" s="5"/>
       <c r="C60" s="6"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="17"/>
+      <c r="E60" s="15"/>
       <c r="F60" s="6"/>
     </row>
     <row r="61" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1588,7 +1528,7 @@
       <c r="B61" s="3"/>
       <c r="C61" s="6"/>
       <c r="D61" s="3"/>
-      <c r="E61" s="16"/>
+      <c r="E61" s="14"/>
       <c r="F61" s="6"/>
     </row>
     <row r="62" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1596,7 +1536,7 @@
       <c r="B62" s="5"/>
       <c r="C62" s="6"/>
       <c r="D62" s="5"/>
-      <c r="E62" s="17"/>
+      <c r="E62" s="15"/>
       <c r="F62" s="6"/>
     </row>
     <row r="63" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1604,7 +1544,7 @@
       <c r="B63" s="3"/>
       <c r="C63" s="6"/>
       <c r="D63" s="3"/>
-      <c r="E63" s="16"/>
+      <c r="E63" s="14"/>
       <c r="F63" s="6"/>
     </row>
     <row r="64" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1612,7 +1552,7 @@
       <c r="B64" s="5"/>
       <c r="C64" s="6"/>
       <c r="D64" s="5"/>
-      <c r="E64" s="17"/>
+      <c r="E64" s="15"/>
       <c r="F64" s="6"/>
     </row>
     <row r="65" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1620,7 +1560,7 @@
       <c r="B65" s="3"/>
       <c r="C65" s="6"/>
       <c r="D65" s="3"/>
-      <c r="E65" s="16"/>
+      <c r="E65" s="14"/>
       <c r="F65" s="6"/>
     </row>
     <row r="66" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1628,7 +1568,7 @@
       <c r="B66" s="5"/>
       <c r="C66" s="6"/>
       <c r="D66" s="5"/>
-      <c r="E66" s="17"/>
+      <c r="E66" s="15"/>
       <c r="F66" s="6"/>
     </row>
     <row r="67" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1636,7 +1576,7 @@
       <c r="B67" s="3"/>
       <c r="C67" s="6"/>
       <c r="D67" s="3"/>
-      <c r="E67" s="16"/>
+      <c r="E67" s="14"/>
       <c r="F67" s="6"/>
     </row>
     <row r="68" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1644,7 +1584,7 @@
       <c r="B68" s="5"/>
       <c r="C68" s="6"/>
       <c r="D68" s="5"/>
-      <c r="E68" s="17"/>
+      <c r="E68" s="15"/>
       <c r="F68" s="6"/>
     </row>
     <row r="69" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1652,7 +1592,7 @@
       <c r="B69" s="3"/>
       <c r="C69" s="6"/>
       <c r="D69" s="3"/>
-      <c r="E69" s="16"/>
+      <c r="E69" s="14"/>
       <c r="F69" s="6"/>
     </row>
     <row r="70" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1660,7 +1600,7 @@
       <c r="B70" s="5"/>
       <c r="C70" s="6"/>
       <c r="D70" s="5"/>
-      <c r="E70" s="17"/>
+      <c r="E70" s="15"/>
       <c r="F70" s="6"/>
     </row>
     <row r="71" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1668,7 +1608,7 @@
       <c r="B71" s="3"/>
       <c r="C71" s="6"/>
       <c r="D71" s="3"/>
-      <c r="E71" s="16"/>
+      <c r="E71" s="14"/>
       <c r="F71" s="6"/>
     </row>
     <row r="72" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1676,7 +1616,7 @@
       <c r="B72" s="5"/>
       <c r="C72" s="6"/>
       <c r="D72" s="5"/>
-      <c r="E72" s="17"/>
+      <c r="E72" s="15"/>
       <c r="F72" s="6"/>
     </row>
     <row r="73" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1684,7 +1624,7 @@
       <c r="B73" s="3"/>
       <c r="C73" s="6"/>
       <c r="D73" s="3"/>
-      <c r="E73" s="16"/>
+      <c r="E73" s="14"/>
       <c r="F73" s="6"/>
     </row>
     <row r="74" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1692,7 +1632,7 @@
       <c r="B74" s="5"/>
       <c r="C74" s="6"/>
       <c r="D74" s="5"/>
-      <c r="E74" s="17"/>
+      <c r="E74" s="15"/>
       <c r="F74" s="6"/>
     </row>
     <row r="75" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1700,40 +1640,8 @@
       <c r="B75" s="3"/>
       <c r="C75" s="6"/>
       <c r="D75" s="3"/>
-      <c r="E75" s="16"/>
+      <c r="E75" s="14"/>
       <c r="F75" s="6"/>
-    </row>
-    <row r="76" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A76" s="6"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="6"/>
-    </row>
-    <row r="77" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A77" s="6"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="16"/>
-      <c r="F77" s="6"/>
-    </row>
-    <row r="78" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A78" s="6"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="6"/>
-    </row>
-    <row r="79" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A79" s="6"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="16"/>
-      <c r="F79" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>